<commit_message>
Picture height and width
</commit_message>
<xml_diff>
--- a/datasets/JSON_gen.xlsx
+++ b/datasets/JSON_gen.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Height</t>
   </si>
   <si>
     <t xml:space="preserve">Topic</t>
@@ -141,7 +147,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -163,12 +169,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,7 +222,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -243,22 +243,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.45"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -277,225 +277,297 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>45363</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>45364</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>45365</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>45366</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>45367</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>45368</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>24</v>
+        <v>11</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>45369</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>45370</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>45371</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>45372</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>33</v>
+        <v>11</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>45373</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>36</v>
+        <v>11</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>